<commit_message>
Increase the seconds of currency drop-down to become present in test.py for 'js-currency-sort-footer'
</commit_message>
<xml_diff>
--- a/TestReports_All.xlsx
+++ b/TestReports_All.xlsx
@@ -529,12 +529,12 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Fail</t>
+          <t>Pass</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>2 broken links found</t>
+          <t>No broken links found</t>
         </is>
       </c>
     </row>
@@ -593,7 +593,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -615,40 +615,6 @@
       <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Comments</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
-      <c r="A2" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/StaysTravel</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Request error: HTTPSConnectionPool(host='www.facebook.com', port=443): Max retries exceeded with url: /StaysTravel (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x7c13e504ade0&gt;: Failed to resolve 'www.facebook.com' ([Errno -3] Temporary failure in name resolution)"))</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="inlineStr">
-        <is>
-          <t>https://www.facebook.com/StaysTravel</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t>Fail</t>
-        </is>
-      </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Request error: HTTPSConnectionPool(host='www.facebook.com', port=443): Max retries exceeded with url: /StaysTravel (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x7c13e504a990&gt;: Failed to resolve 'www.facebook.com' ([Errno -3] Temporary failure in name resolution)"))</t>
         </is>
       </c>
     </row>
@@ -8856,7 +8822,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>182.160.106.203</t>
+          <t>43.250.81.50</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
in test.py writing workbook.save()  after every tests
</commit_message>
<xml_diff>
--- a/TestReports_All.xlsx
+++ b/TestReports_All.xlsx
@@ -631,7 +631,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Request error: HTTPSConnectionPool(host='www.facebook.com', port=443): Max retries exceeded with url: /StaysTravel (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x7e84b8258a70&gt;: Failed to resolve 'www.facebook.com' ([Errno -3] Temporary failure in name resolution)"))</t>
+          <t>Request error: HTTPSConnectionPool(host='www.facebook.com', port=443): Max retries exceeded with url: /StaysTravel (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x76d75d247e60&gt;: Failed to resolve 'www.facebook.com' ([Errno -3] Temporary failure in name resolution)"))</t>
         </is>
       </c>
     </row>
@@ -648,7 +648,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Request error: HTTPSConnectionPool(host='www.facebook.com', port=443): Max retries exceeded with url: /StaysTravel (Caused by SSLError(SSLError(1, '[SSL] unknown error (_ssl.c:1000)')))</t>
+          <t>Request error: HTTPSConnectionPool(host='www.facebook.com', port=443): Max retries exceeded with url: /StaysTravel (Caused by NameResolutionError("&lt;urllib3.connection.HTTPSConnection object at 0x76d75d2476e0&gt;: Failed to resolve 'www.facebook.com' ([Errno -3] Temporary failure in name resolution)"))</t>
         </is>
       </c>
     </row>

</xml_diff>